<commit_message>
Added fdir_results to tm59 and tm59mechvent to override output path of report. Created tm59 test
</commit_message>
<xml_diff>
--- a/tests/testmodels/TestJob1/mf_results/tm59/TM59__TestJob1.xlsx
+++ b/tests/testmodels/TestJob1/mf_results/tm59/TM59__TestJob1.xlsx
@@ -27,18 +27,18 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1571" uniqueCount="127">
   <si>
+    <t>sheet_name</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
     <t>JobNo</t>
   </si>
   <si>
     <t>Date</t>
   </si>
   <si>
-    <t>sheet_name</t>
-  </si>
-  <si>
-    <t>Author</t>
-  </si>
-  <si>
     <t>0</t>
   </si>
   <si>
@@ -72,12 +72,6 @@
     <t>10</t>
   </si>
   <si>
-    <t>ngDe</t>
-  </si>
-  <si>
-    <t>20220303</t>
-  </si>
-  <si>
     <t>Project Information</t>
   </si>
   <si>
@@ -111,7 +105,13 @@
     <t>Results, Air Speed 0.8</t>
   </si>
   <si>
-    <t>O.Hensby</t>
+    <t>jovyan</t>
+  </si>
+  <si>
+    <t>/c/e</t>
+  </si>
+  <si>
+    <t>20220304</t>
   </si>
   <si>
     <t>index</t>
@@ -177,7 +177,7 @@
     <t>51.38</t>
   </si>
   <si>
-    <t>2022-03-03 16:23:11.827513</t>
+    <t>2022-03-04 17:31:00.947870</t>
   </si>
   <si>
     <t>2021.4.0.0</t>
@@ -412,7 +412,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -423,14 +423,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -493,7 +485,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -597,10 +589,10 @@
   <autoFilter ref="A1:E12"/>
   <tableColumns count="5">
     <tableColumn id="1" name="index"/>
-    <tableColumn id="2" name="JobNo"/>
-    <tableColumn id="3" name="Date"/>
-    <tableColumn id="4" name="sheet_name"/>
-    <tableColumn id="5" name="Author"/>
+    <tableColumn id="2" name="sheet_name"/>
+    <tableColumn id="3" name="Author"/>
+    <tableColumn id="4" name="JobNo"/>
+    <tableColumn id="5" name="Date"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -620,7 +612,7 @@
     <tableColumn id="8" name="Criterion 2 (Pass/Fail)"/>
     <tableColumn id="9" name="TM59 (Pass/Fail)"/>
   </tableColumns>
-  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -638,7 +630,7 @@
     <tableColumn id="8" name="Criterion 2 (Pass/Fail)"/>
     <tableColumn id="9" name="TM59 (Pass/Fail)"/>
   </tableColumns>
-  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -656,7 +648,7 @@
     <tableColumn id="8" name="Criterion 2 (Pass/Fail)"/>
     <tableColumn id="9" name="TM59 (Pass/Fail)"/>
   </tableColumns>
-  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -667,7 +659,7 @@
     <tableColumn id="1" name="index"/>
     <tableColumn id="2" name="Information"/>
   </tableColumns>
-  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -678,7 +670,7 @@
     <tableColumn id="1" name="index"/>
     <tableColumn id="2" name="Definition"/>
   </tableColumns>
-  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -696,7 +688,7 @@
     <tableColumn id="8" name="Criterion 2 (Pass/Fail)"/>
     <tableColumn id="9" name="TM59 (Pass/Fail)"/>
   </tableColumns>
-  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -714,7 +706,7 @@
     <tableColumn id="8" name="Criterion 2 (Pass/Fail)"/>
     <tableColumn id="9" name="TM59 (Pass/Fail)"/>
   </tableColumns>
-  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -732,7 +724,7 @@
     <tableColumn id="8" name="Criterion 2 (Pass/Fail)"/>
     <tableColumn id="9" name="TM59 (Pass/Fail)"/>
   </tableColumns>
-  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -750,7 +742,7 @@
     <tableColumn id="8" name="Criterion 2 (Pass/Fail)"/>
     <tableColumn id="9" name="TM59 (Pass/Fail)"/>
   </tableColumns>
-  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -768,7 +760,7 @@
     <tableColumn id="8" name="Criterion 2 (Pass/Fail)"/>
     <tableColumn id="9" name="TM59 (Pass/Fail)"/>
   </tableColumns>
-  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -786,7 +778,7 @@
     <tableColumn id="8" name="Criterion 2 (Pass/Fail)"/>
     <tableColumn id="9" name="TM59 (Pass/Fail)"/>
   </tableColumns>
-  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1115,10 +1107,10 @@
         <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>28</v>
@@ -1129,13 +1121,13 @@
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>28</v>
@@ -1146,13 +1138,13 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>28</v>
@@ -1163,13 +1155,13 @@
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>28</v>
@@ -1180,13 +1172,13 @@
         <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>28</v>
@@ -1197,13 +1189,13 @@
         <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>28</v>
@@ -1214,13 +1206,13 @@
         <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>28</v>
@@ -1231,13 +1223,13 @@
         <v>11</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>28</v>
@@ -1248,13 +1240,13 @@
         <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>28</v>
@@ -1265,13 +1257,13 @@
         <v>13</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>28</v>
@@ -1282,10 +1274,10 @@
         <v>14</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>27</v>
@@ -1660,7 +1652,7 @@
         <v>125</v>
       </c>
       <c r="G13">
-        <v>9.8</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="H13" t="s">
         <v>126</v>
@@ -1747,7 +1739,7 @@
         <v>125</v>
       </c>
       <c r="G16">
-        <v>9.8</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="H16" t="s">
         <v>126</v>
@@ -2100,7 +2092,7 @@
         <v>125</v>
       </c>
       <c r="G29">
-        <v>8.3</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="H29" t="s">
         <v>126</v>
@@ -2187,7 +2179,7 @@
         <v>125</v>
       </c>
       <c r="G32">
-        <v>8.3</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="H32" t="s">
         <v>126</v>
@@ -2561,7 +2553,7 @@
         <v>125</v>
       </c>
       <c r="G13">
-        <v>9.8</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="H13" t="s">
         <v>126</v>
@@ -2648,7 +2640,7 @@
         <v>125</v>
       </c>
       <c r="G16">
-        <v>9.7</v>
+        <v>9.699999999999999</v>
       </c>
       <c r="H16" t="s">
         <v>126</v>
@@ -3001,7 +2993,7 @@
         <v>125</v>
       </c>
       <c r="G29">
-        <v>8.3</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="H29" t="s">
         <v>126</v>
@@ -3088,7 +3080,7 @@
         <v>125</v>
       </c>
       <c r="G32">
-        <v>8.3</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="H32" t="s">
         <v>126</v>
@@ -3462,7 +3454,7 @@
         <v>125</v>
       </c>
       <c r="G13">
-        <v>9.8</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="H13" t="s">
         <v>126</v>
@@ -3549,7 +3541,7 @@
         <v>125</v>
       </c>
       <c r="G16">
-        <v>9.7</v>
+        <v>9.699999999999999</v>
       </c>
       <c r="H16" t="s">
         <v>126</v>
@@ -3902,7 +3894,7 @@
         <v>125</v>
       </c>
       <c r="G29">
-        <v>8.3</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="H29" t="s">
         <v>126</v>
@@ -3989,7 +3981,7 @@
         <v>125</v>
       </c>
       <c r="G32">
-        <v>8.3</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="H32" t="s">
         <v>126</v>
@@ -4609,7 +4601,7 @@
         <v>125</v>
       </c>
       <c r="G16">
-        <v>9.8</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="H16" t="s">
         <v>126</v>
@@ -4962,7 +4954,7 @@
         <v>125</v>
       </c>
       <c r="G29">
-        <v>8.3</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="H29" t="s">
         <v>126</v>
@@ -5049,7 +5041,7 @@
         <v>125</v>
       </c>
       <c r="G32">
-        <v>8.3</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="H32" t="s">
         <v>126</v>
@@ -5510,7 +5502,7 @@
         <v>125</v>
       </c>
       <c r="G16">
-        <v>9.8</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="H16" t="s">
         <v>126</v>
@@ -5863,7 +5855,7 @@
         <v>125</v>
       </c>
       <c r="G29">
-        <v>8.3</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="H29" t="s">
         <v>126</v>
@@ -5950,7 +5942,7 @@
         <v>125</v>
       </c>
       <c r="G32">
-        <v>8.3</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="H32" t="s">
         <v>126</v>
@@ -6324,7 +6316,7 @@
         <v>125</v>
       </c>
       <c r="G13">
-        <v>9.8</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="H13" t="s">
         <v>126</v>
@@ -6411,7 +6403,7 @@
         <v>125</v>
       </c>
       <c r="G16">
-        <v>9.8</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="H16" t="s">
         <v>126</v>
@@ -6463,7 +6455,7 @@
         <v>0</v>
       </c>
       <c r="E18">
-        <v>8.2</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="F18" t="s">
         <v>126</v>
@@ -6515,7 +6507,7 @@
         <v>0</v>
       </c>
       <c r="E20">
-        <v>8.2</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="F20" t="s">
         <v>126</v>
@@ -6764,7 +6756,7 @@
         <v>125</v>
       </c>
       <c r="G29">
-        <v>8.3</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="H29" t="s">
         <v>126</v>
@@ -6851,7 +6843,7 @@
         <v>125</v>
       </c>
       <c r="G32">
-        <v>8.3</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="H32" t="s">
         <v>126</v>
@@ -7225,7 +7217,7 @@
         <v>125</v>
       </c>
       <c r="G13">
-        <v>9.8</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="H13" t="s">
         <v>126</v>
@@ -7312,7 +7304,7 @@
         <v>125</v>
       </c>
       <c r="G16">
-        <v>9.8</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="H16" t="s">
         <v>126</v>
@@ -7665,7 +7657,7 @@
         <v>125</v>
       </c>
       <c r="G29">
-        <v>8.3</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="H29" t="s">
         <v>126</v>
@@ -7752,7 +7744,7 @@
         <v>125</v>
       </c>
       <c r="G32">
-        <v>8.3</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="H32" t="s">
         <v>126</v>
@@ -8126,7 +8118,7 @@
         <v>125</v>
       </c>
       <c r="G13">
-        <v>9.8</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="H13" t="s">
         <v>126</v>
@@ -8213,7 +8205,7 @@
         <v>125</v>
       </c>
       <c r="G16">
-        <v>9.8</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="H16" t="s">
         <v>126</v>
@@ -8566,7 +8558,7 @@
         <v>125</v>
       </c>
       <c r="G29">
-        <v>8.3</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="H29" t="s">
         <v>126</v>
@@ -8653,7 +8645,7 @@
         <v>125</v>
       </c>
       <c r="G32">
-        <v>8.3</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="H32" t="s">
         <v>126</v>
@@ -9027,7 +9019,7 @@
         <v>125</v>
       </c>
       <c r="G13">
-        <v>9.8</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="H13" t="s">
         <v>126</v>
@@ -9114,7 +9106,7 @@
         <v>125</v>
       </c>
       <c r="G16">
-        <v>9.8</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="H16" t="s">
         <v>126</v>
@@ -9467,7 +9459,7 @@
         <v>125</v>
       </c>
       <c r="G29">
-        <v>8.3</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="H29" t="s">
         <v>126</v>
@@ -9554,7 +9546,7 @@
         <v>125</v>
       </c>
       <c r="G32">
-        <v>8.3</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="H32" t="s">
         <v>126</v>

</xml_diff>

<commit_message>
Removed datamine_functions.py. Any funcs in use have been moved to utils.py
</commit_message>
<xml_diff>
--- a/tests/testmodels/TestJob1/mf_results/tm59/TM59__TestJob1.xlsx
+++ b/tests/testmodels/TestJob1/mf_results/tm59/TM59__TestJob1.xlsx
@@ -27,18 +27,18 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1584" uniqueCount="131">
   <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>JobNo</t>
+  </si>
+  <si>
     <t>sheet_name</t>
   </si>
   <si>
     <t>Date</t>
   </si>
   <si>
-    <t>JobNo</t>
-  </si>
-  <si>
-    <t>Author</t>
-  </si>
-  <si>
     <t>0</t>
   </si>
   <si>
@@ -72,6 +72,12 @@
     <t>10</t>
   </si>
   <si>
+    <t>jovyan</t>
+  </si>
+  <si>
+    <t>/c/e</t>
+  </si>
+  <si>
     <t>Project Information</t>
   </si>
   <si>
@@ -105,13 +111,7 @@
     <t>Results, Air Speed 0.8</t>
   </si>
   <si>
-    <t>20220325</t>
-  </si>
-  <si>
-    <t>/c/e</t>
-  </si>
-  <si>
-    <t>jovyan</t>
+    <t>20220422</t>
   </si>
   <si>
     <t>index</t>
@@ -183,7 +183,7 @@
     <t>51.38</t>
   </si>
   <si>
-    <t>2022-03-25 19:32:56.180669</t>
+    <t>2022-04-22 12:42:30.496561</t>
   </si>
   <si>
     <t>2021.4.0.0</t>
@@ -601,10 +601,10 @@
   <autoFilter ref="A1:E12"/>
   <tableColumns count="5">
     <tableColumn id="1" name="index"/>
-    <tableColumn id="2" name="sheet_name"/>
-    <tableColumn id="3" name="Date"/>
-    <tableColumn id="4" name="JobNo"/>
-    <tableColumn id="5" name="Author"/>
+    <tableColumn id="2" name="Author"/>
+    <tableColumn id="3" name="JobNo"/>
+    <tableColumn id="4" name="sheet_name"/>
+    <tableColumn id="5" name="Date"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1119,10 +1119,10 @@
         <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>28</v>
@@ -1133,13 +1133,13 @@
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>28</v>
@@ -1150,13 +1150,13 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>28</v>
@@ -1167,13 +1167,13 @@
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>28</v>
@@ -1184,13 +1184,13 @@
         <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>28</v>
@@ -1201,13 +1201,13 @@
         <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>28</v>
@@ -1218,13 +1218,13 @@
         <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>28</v>
@@ -1235,13 +1235,13 @@
         <v>11</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>28</v>
@@ -1252,13 +1252,13 @@
         <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>28</v>
@@ -1269,13 +1269,13 @@
         <v>13</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>28</v>
@@ -1286,10 +1286,10 @@
         <v>14</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>27</v>

</xml_diff>